<commit_message>
Updated the performance for RF::Cyscore
</commit_message>
<xml_diff>
--- a/v2013/Performance/Performance.xlsx
+++ b/v2013/Performance/Performance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacky\Dropbox (LU's Team)\Jacky Lee\Papers\MLSF extended 2.0\PDBbind v2013\Performance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacky\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAD0053-C2BE-4967-B46D-A5EC28702D8B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D1A0CB-FF33-41D5-AA43-CE92C06C973E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{883CA29F-C084-4A6C-A604-84F9538E29DB}"/>
   </bookViews>
@@ -14556,13 +14556,13 @@
         <v>457</v>
       </c>
       <c r="E612" s="7">
-        <v>0.44285189237893402</v>
+        <v>0.48985085884937901</v>
       </c>
       <c r="F612" s="7">
-        <v>0.43668055849404602</v>
+        <v>0.51070847678411901</v>
       </c>
       <c r="G612" s="7">
-        <v>2.04685810343583</v>
+        <v>2.0141205737502301</v>
       </c>
     </row>
     <row r="613" spans="1:7">
@@ -14579,13 +14579,13 @@
         <v>515</v>
       </c>
       <c r="E613" s="7">
-        <v>0.46209395728770702</v>
+        <v>0.50518732304487901</v>
       </c>
       <c r="F613" s="7">
-        <v>0.463601052129331</v>
+        <v>0.52088933861192199</v>
       </c>
       <c r="G613" s="7">
-        <v>2.0361573713555101</v>
+        <v>2.0068619076827101</v>
       </c>
     </row>
     <row r="614" spans="1:7">
@@ -14602,13 +14602,13 @@
         <v>590</v>
       </c>
       <c r="E614" s="7">
-        <v>0.43977071284566999</v>
+        <v>0.50987233793198605</v>
       </c>
       <c r="F614" s="7">
-        <v>0.4525195226905</v>
+        <v>0.52395549277022002</v>
       </c>
       <c r="G614" s="7">
-        <v>2.07704991091054</v>
+        <v>2.0125285868307898</v>
       </c>
     </row>
     <row r="615" spans="1:7">
@@ -14625,13 +14625,13 @@
         <v>642</v>
       </c>
       <c r="E615" s="7">
-        <v>0.45353233497290701</v>
+        <v>0.50824273030091505</v>
       </c>
       <c r="F615" s="7">
-        <v>0.47034756234778702</v>
+        <v>0.52124539768546396</v>
       </c>
       <c r="G615" s="7">
-        <v>2.0531559505402299</v>
+        <v>2.01427731656849</v>
       </c>
     </row>
     <row r="616" spans="1:7">
@@ -14648,13 +14648,13 @@
         <v>689</v>
       </c>
       <c r="E616" s="7">
-        <v>0.44454126035284097</v>
+        <v>0.49532776598752598</v>
       </c>
       <c r="F616" s="7">
-        <v>0.46221323096768402</v>
+        <v>0.50865466330991504</v>
       </c>
       <c r="G616" s="7">
-        <v>2.0744302231196801</v>
+        <v>2.0330407677437998</v>
       </c>
     </row>
     <row r="617" spans="1:7">
@@ -14671,13 +14671,13 @@
         <v>729</v>
       </c>
       <c r="E617" s="7">
-        <v>0.45042291273933999</v>
+        <v>0.50547753227384895</v>
       </c>
       <c r="F617" s="7">
-        <v>0.47390815308320799</v>
+        <v>0.523288691232495</v>
       </c>
       <c r="G617" s="7">
-        <v>2.0655674349306201</v>
+        <v>2.0234314848826598</v>
       </c>
     </row>
     <row r="618" spans="1:7">
@@ -14694,13 +14694,13 @@
         <v>774</v>
       </c>
       <c r="E618" s="7">
-        <v>0.47298945021170802</v>
+        <v>0.513261859064574</v>
       </c>
       <c r="F618" s="7">
-        <v>0.48510863862160902</v>
+        <v>0.52561602281319297</v>
       </c>
       <c r="G618" s="7">
-        <v>2.0256135702792601</v>
+        <v>1.9953269195124801</v>
       </c>
     </row>
     <row r="619" spans="1:7">
@@ -14717,13 +14717,13 @@
         <v>817</v>
       </c>
       <c r="E619" s="7">
-        <v>0.45845842301114598</v>
+        <v>0.50782532663094104</v>
       </c>
       <c r="F619" s="7">
-        <v>0.47052963801039399</v>
+        <v>0.51643374484164295</v>
       </c>
       <c r="G619" s="7">
-        <v>2.0331971479973201</v>
+        <v>1.9879478327390001</v>
       </c>
     </row>
     <row r="620" spans="1:7">
@@ -14740,13 +14740,13 @@
         <v>848</v>
       </c>
       <c r="E620" s="7">
-        <v>0.45076624023747502</v>
+        <v>0.50245861133584901</v>
       </c>
       <c r="F620" s="7">
-        <v>0.458708476768796</v>
+        <v>0.50589115936412798</v>
       </c>
       <c r="G620" s="7">
-        <v>2.03822321287943</v>
+        <v>1.9903424590130301</v>
       </c>
     </row>
     <row r="621" spans="1:7">
@@ -14763,13 +14763,13 @@
         <v>867</v>
       </c>
       <c r="E621" s="7">
-        <v>0.43884007298942002</v>
+        <v>0.49223873453281702</v>
       </c>
       <c r="F621" s="7">
-        <v>0.450357273043899</v>
+        <v>0.49635605921970399</v>
       </c>
       <c r="G621" s="7">
-        <v>2.0506268198843101</v>
+        <v>1.9995657019411399</v>
       </c>
     </row>
     <row r="622" spans="1:7">
@@ -14786,13 +14786,13 @@
         <v>889</v>
       </c>
       <c r="E622" s="7">
-        <v>0.45431565490970099</v>
+        <v>0.496847552399445</v>
       </c>
       <c r="F622" s="7">
-        <v>0.46643738634016102</v>
+        <v>0.49762977963278399</v>
       </c>
       <c r="G622" s="7">
-        <v>2.0313870178954199</v>
+        <v>1.9917420377930699</v>
       </c>
     </row>
     <row r="623" spans="1:7">
@@ -14809,13 +14809,13 @@
         <v>908</v>
       </c>
       <c r="E623" s="7">
-        <v>0.46199252857914502</v>
+        <v>0.50488669968921196</v>
       </c>
       <c r="F623" s="7">
-        <v>0.47416548668635899</v>
+        <v>0.52089662163842598</v>
       </c>
       <c r="G623" s="7">
-        <v>2.01884067936337</v>
+        <v>1.98212409744478</v>
       </c>
     </row>
     <row r="624" spans="1:7">
@@ -14832,13 +14832,13 @@
         <v>922</v>
       </c>
       <c r="E624" s="7">
-        <v>0.45315521540368597</v>
+        <v>0.50510293822700003</v>
       </c>
       <c r="F624" s="7">
-        <v>0.46413109461380903</v>
+        <v>0.51586081342330703</v>
       </c>
       <c r="G624" s="7">
-        <v>2.0306581641757</v>
+        <v>1.98012452156226</v>
       </c>
     </row>
     <row r="625" spans="1:7">
@@ -14855,13 +14855,13 @@
         <v>941</v>
       </c>
       <c r="E625" s="7">
-        <v>0.43946967978544199</v>
+        <v>0.50775998849903303</v>
       </c>
       <c r="F625" s="7">
-        <v>0.45079668230965703</v>
+        <v>0.51245802159547804</v>
       </c>
       <c r="G625" s="7">
-        <v>2.0462467904531398</v>
+        <v>1.97429373004709</v>
       </c>
     </row>
     <row r="626" spans="1:7">
@@ -14878,13 +14878,13 @@
         <v>954</v>
       </c>
       <c r="E626" s="7">
-        <v>0.44676407158242398</v>
+        <v>0.50616737346710095</v>
       </c>
       <c r="F626" s="7">
-        <v>0.44973012353936498</v>
+        <v>0.50810762709692703</v>
       </c>
       <c r="G626" s="7">
-        <v>2.0329735260845299</v>
+        <v>1.9748657303549999</v>
       </c>
     </row>
     <row r="627" spans="1:7">
@@ -14901,13 +14901,13 @@
         <v>981</v>
       </c>
       <c r="E627" s="7">
-        <v>0.45504452004047902</v>
+        <v>0.50869970964867295</v>
       </c>
       <c r="F627" s="7">
-        <v>0.46126643752212898</v>
+        <v>0.51541331190587802</v>
       </c>
       <c r="G627" s="7">
-        <v>2.0211424575116901</v>
+        <v>1.96999796795076</v>
       </c>
     </row>
     <row r="628" spans="1:7">
@@ -14924,13 +14924,13 @@
         <v>995</v>
       </c>
       <c r="E628" s="7">
-        <v>0.43925539868640601</v>
+        <v>0.51011225901845203</v>
       </c>
       <c r="F628" s="7">
-        <v>0.45489378933089197</v>
+        <v>0.52101719618832998</v>
       </c>
       <c r="G628" s="7">
-        <v>2.04110292473852</v>
+        <v>1.9695613415439499</v>
       </c>
     </row>
     <row r="629" spans="1:7">
@@ -14947,13 +14947,13 @@
         <v>1005</v>
       </c>
       <c r="E629" s="7">
-        <v>0.45128914440682</v>
+        <v>0.50594960356640994</v>
       </c>
       <c r="F629" s="7">
-        <v>0.46952134345213598</v>
+        <v>0.51670564449780199</v>
       </c>
       <c r="G629" s="7">
-        <v>2.0273817036300699</v>
+        <v>1.9728735659460199</v>
       </c>
     </row>
     <row r="630" spans="1:7">
@@ -14970,13 +14970,13 @@
         <v>1034</v>
       </c>
       <c r="E630" s="7">
-        <v>0.45426657109444402</v>
+        <v>0.52030390492765999</v>
       </c>
       <c r="F630" s="7">
-        <v>0.46767307317038498</v>
+        <v>0.52724094694881296</v>
       </c>
       <c r="G630" s="7">
-        <v>2.0242145714333302</v>
+        <v>1.9623589208285701</v>
       </c>
     </row>
     <row r="631" spans="1:7">
@@ -14993,13 +14993,13 @@
         <v>1059</v>
       </c>
       <c r="E631" s="7">
-        <v>0.45233917366325699</v>
+        <v>0.52005433828381298</v>
       </c>
       <c r="F631" s="7">
-        <v>0.465038236026174</v>
+        <v>0.52900263013767901</v>
       </c>
       <c r="G631" s="7">
-        <v>2.0252282819241199</v>
+        <v>1.9606590719852099</v>
       </c>
     </row>
     <row r="632" spans="1:7">
@@ -15016,13 +15016,13 @@
         <v>1073</v>
       </c>
       <c r="E632" s="7">
-        <v>0.45655087499958502</v>
+        <v>0.52271646905281</v>
       </c>
       <c r="F632" s="7">
-        <v>0.46643010331365697</v>
+        <v>0.52755088018782803</v>
       </c>
       <c r="G632" s="7">
-        <v>2.02027110622064</v>
+        <v>1.9572598979737601</v>
       </c>
     </row>
     <row r="633" spans="1:7">
@@ -15039,13 +15039,13 @@
         <v>1117</v>
       </c>
       <c r="E633" s="7">
-        <v>0.45103475106651802</v>
+        <v>0.50548142755705305</v>
       </c>
       <c r="F633" s="7">
-        <v>0.46832207175443302</v>
+        <v>0.51356018627312405</v>
       </c>
       <c r="G633" s="7">
-        <v>2.02555401710543</v>
+        <v>1.97629326154664</v>
       </c>
     </row>
     <row r="634" spans="1:7">
@@ -15062,13 +15062,13 @@
         <v>1125</v>
       </c>
       <c r="E634" s="7">
-        <v>0.45622165419281002</v>
+        <v>0.51112019002569598</v>
       </c>
       <c r="F634" s="7">
-        <v>0.466665587837295</v>
+        <v>0.51995063741803804</v>
       </c>
       <c r="G634" s="7">
-        <v>2.01452856830287</v>
+        <v>1.96804967727497</v>
       </c>
     </row>
     <row r="635" spans="1:7">
@@ -15085,13 +15085,13 @@
         <v>1135</v>
       </c>
       <c r="E635" s="7">
-        <v>0.46003039534427398</v>
+        <v>0.51529892186639803</v>
       </c>
       <c r="F635" s="7">
-        <v>0.47081367604405999</v>
+        <v>0.52371677134591299</v>
       </c>
       <c r="G635" s="7">
-        <v>2.0073663205105299</v>
+        <v>1.9629596719545499</v>
       </c>
     </row>
     <row r="636" spans="1:7">
@@ -15108,13 +15108,13 @@
         <v>1167</v>
       </c>
       <c r="E636" s="7">
-        <v>0.47455562943531399</v>
+        <v>0.52613089435548799</v>
       </c>
       <c r="F636" s="7">
-        <v>0.49961238129227997</v>
+        <v>0.53986566878138198</v>
       </c>
       <c r="G636" s="7">
-        <v>1.99274234511969</v>
+        <v>1.9543950197995199</v>
       </c>
     </row>
     <row r="637" spans="1:7">
@@ -15131,13 +15131,13 @@
         <v>1184</v>
       </c>
       <c r="E637" s="7">
-        <v>0.454531592977796</v>
+        <v>0.51889477239303605</v>
       </c>
       <c r="F637" s="7">
-        <v>0.47430629186544099</v>
+        <v>0.52986688261618597</v>
       </c>
       <c r="G637" s="7">
-        <v>2.0154846493187901</v>
+        <v>1.96361334426104</v>
       </c>
     </row>
     <row r="638" spans="1:7">
@@ -15154,13 +15154,13 @@
         <v>1198</v>
       </c>
       <c r="E638" s="7">
-        <v>0.46978687187988599</v>
+        <v>0.52794781140272196</v>
       </c>
       <c r="F638" s="7">
-        <v>0.48042646180453003</v>
+        <v>0.53561885510422502</v>
       </c>
       <c r="G638" s="7">
-        <v>1.99745107448201</v>
+        <v>1.9563130018027499</v>
       </c>
     </row>
     <row r="639" spans="1:7">
@@ -15177,13 +15177,13 @@
         <v>1207</v>
       </c>
       <c r="E639" s="7">
-        <v>0.47925779109814998</v>
+        <v>0.52908851546359403</v>
       </c>
       <c r="F639" s="7">
-        <v>0.49948452371587099</v>
+        <v>0.54324094695352798</v>
       </c>
       <c r="G639" s="7">
-        <v>1.9877816257998999</v>
+        <v>1.95108169026957</v>
       </c>
     </row>
     <row r="640" spans="1:7">
@@ -15200,13 +15200,13 @@
         <v>1223</v>
       </c>
       <c r="E640" s="7">
-        <v>0.46269806878605002</v>
+        <v>0.52618290662481104</v>
       </c>
       <c r="F640" s="7">
-        <v>0.47779567078615398</v>
+        <v>0.53639975739051604</v>
       </c>
       <c r="G640" s="7">
-        <v>2.00499670151315</v>
+        <v>1.9523005261281501</v>
       </c>
     </row>
     <row r="641" spans="1:7">
@@ -15223,13 +15223,13 @@
         <v>1238</v>
       </c>
       <c r="E641" s="7">
-        <v>0.48610182951256398</v>
+        <v>0.53933123959927498</v>
       </c>
       <c r="F641" s="7">
-        <v>0.50148330987871004</v>
+        <v>0.553165284403347</v>
       </c>
       <c r="G641" s="7">
-        <v>1.9807103744257899</v>
+        <v>1.9409208654588701</v>
       </c>
     </row>
     <row r="642" spans="1:7">
@@ -15246,13 +15246,13 @@
         <v>1243</v>
       </c>
       <c r="E642" s="7">
-        <v>0.47500078271957902</v>
+        <v>0.53682201657850104</v>
       </c>
       <c r="F642" s="7">
-        <v>0.49390410696326598</v>
+        <v>0.54780902302203904</v>
       </c>
       <c r="G642" s="7">
-        <v>1.9923583308847199</v>
+        <v>1.9436676803538799</v>
       </c>
     </row>
     <row r="643" spans="1:7">
@@ -15269,13 +15269,13 @@
         <v>1244</v>
       </c>
       <c r="E643" s="7">
-        <v>0.492148353295772</v>
+        <v>0.53302418401603802</v>
       </c>
       <c r="F643" s="7">
-        <v>0.51568035621103403</v>
+        <v>0.54016265441772304</v>
       </c>
       <c r="G643" s="7">
-        <v>1.97187332228617</v>
+        <v>1.9446522260438099</v>
       </c>
     </row>
     <row r="644" spans="1:7">
@@ -15292,13 +15292,13 @@
         <v>1246</v>
       </c>
       <c r="E644" s="7">
-        <v>0.47553436122918102</v>
+        <v>0.53221922119304099</v>
       </c>
       <c r="F644" s="7">
-        <v>0.49224034001962402</v>
+        <v>0.538507788950919</v>
       </c>
       <c r="G644" s="7">
-        <v>1.9909035801093899</v>
+        <v>1.94740666494654</v>
       </c>
     </row>
     <row r="645" spans="1:7">
@@ -15315,13 +15315,13 @@
         <v>1246</v>
       </c>
       <c r="E645" s="7">
-        <v>0.47553436122918102</v>
+        <v>0.53221922119304099</v>
       </c>
       <c r="F645" s="7">
-        <v>0.49224034001962402</v>
+        <v>0.538507788950919</v>
       </c>
       <c r="G645" s="7">
-        <v>1.9909035801093899</v>
+        <v>1.94740666494654</v>
       </c>
     </row>
     <row r="646" spans="1:7">
@@ -15338,13 +15338,13 @@
         <v>1250</v>
       </c>
       <c r="E646" s="7">
-        <v>0.483616174588894</v>
+        <v>0.53582391458963496</v>
       </c>
       <c r="F646" s="7">
-        <v>0.49818328964710801</v>
+        <v>0.54766659939262297</v>
       </c>
       <c r="G646" s="7">
-        <v>1.98326804451626</v>
+        <v>1.9420154082868899</v>
       </c>
     </row>
     <row r="647" spans="1:7">
@@ -15361,13 +15361,13 @@
         <v>1256</v>
       </c>
       <c r="E647" s="7">
-        <v>0.47512871103158899</v>
+        <v>0.53798106218598996</v>
       </c>
       <c r="F647" s="7">
-        <v>0.49258426071565897</v>
+        <v>0.54556666008389099</v>
       </c>
       <c r="G647" s="7">
-        <v>1.99270402274317</v>
+        <v>1.93909530819031</v>
       </c>
     </row>
     <row r="648" spans="1:7">
@@ -15384,13 +15384,13 @@
         <v>1260</v>
       </c>
       <c r="E648" s="7">
-        <v>0.47514496024398201</v>
+        <v>0.53307698669463699</v>
       </c>
       <c r="F648" s="7">
-        <v>0.49502407459458903</v>
+        <v>0.548112482459717</v>
       </c>
       <c r="G648" s="7">
-        <v>1.9904536328568401</v>
+        <v>1.9445248013544301</v>
       </c>
     </row>
     <row r="649" spans="1:7">
@@ -15407,13 +15407,13 @@
         <v>1277</v>
       </c>
       <c r="E649" s="7">
-        <v>0.46566715617396598</v>
+        <v>0.54192945906754197</v>
       </c>
       <c r="F649" s="7">
-        <v>0.489337649345088</v>
+        <v>0.55243293562708395</v>
       </c>
       <c r="G649" s="7">
-        <v>2.0011524833599501</v>
+        <v>1.9357558283590599</v>
       </c>
     </row>
     <row r="650" spans="1:7">
@@ -15430,13 +15430,13 @@
         <v>1286</v>
       </c>
       <c r="E650" s="7">
-        <v>0.46695088166110799</v>
+        <v>0.53208117426621404</v>
       </c>
       <c r="F650" s="7">
-        <v>0.492114910118717</v>
+        <v>0.54758082152490595</v>
       </c>
       <c r="G650" s="7">
-        <v>2.0003197981243601</v>
+        <v>1.94104875025051</v>
       </c>
     </row>
     <row r="651" spans="1:7">
@@ -15453,13 +15453,13 @@
         <v>1294</v>
       </c>
       <c r="E651" s="7">
-        <v>0.48280594493177698</v>
+        <v>0.53907026455169604</v>
       </c>
       <c r="F651" s="7">
-        <v>0.49907991113230099</v>
+        <v>0.55508719417530705</v>
       </c>
       <c r="G651" s="7">
-        <v>1.9822963252450401</v>
+        <v>1.9353526166969599</v>
       </c>
     </row>
     <row r="652" spans="1:7">
@@ -15476,13 +15476,13 @@
         <v>1303</v>
       </c>
       <c r="E652" s="7">
-        <v>0.487999906769853</v>
+        <v>0.53960998951418804</v>
       </c>
       <c r="F652" s="7">
-        <v>0.50416912820845095</v>
+        <v>0.55054663176247798</v>
       </c>
       <c r="G652" s="7">
-        <v>1.9743188376496501</v>
+        <v>1.93140251994032</v>
       </c>
     </row>
     <row r="653" spans="1:7">
@@ -15499,13 +15499,13 @@
         <v>1309</v>
       </c>
       <c r="E653" s="7">
-        <v>0.490862156369549</v>
+        <v>0.54242707115294797</v>
       </c>
       <c r="F653" s="7">
-        <v>0.51272425667546795</v>
+        <v>0.55529678349359701</v>
       </c>
       <c r="G653" s="7">
-        <v>1.9714570919710599</v>
+        <v>1.9290125214998399</v>
       </c>
     </row>
     <row r="654" spans="1:7">
@@ -15522,13 +15522,13 @@
         <v>1321</v>
       </c>
       <c r="E654" s="7">
-        <v>0.47593436549403301</v>
+        <v>0.538072764090891</v>
       </c>
       <c r="F654" s="7">
-        <v>0.49680841608813497</v>
+        <v>0.55086465725316403</v>
       </c>
       <c r="G654" s="7">
-        <v>1.9862765892994201</v>
+        <v>1.93160173664006</v>
       </c>
     </row>
     <row r="655" spans="1:7">
@@ -15545,13 +15545,13 @@
         <v>1336</v>
       </c>
       <c r="E655" s="7">
-        <v>0.482986895683783</v>
+        <v>0.54484183183128998</v>
       </c>
       <c r="F655" s="7">
-        <v>0.50003560605469399</v>
+        <v>0.55929516504444099</v>
       </c>
       <c r="G655" s="7">
-        <v>1.9787460203345799</v>
+        <v>1.9258268789975701</v>
       </c>
     </row>
     <row r="656" spans="1:7">
@@ -15568,13 +15568,13 @@
         <v>1360</v>
       </c>
       <c r="E656" s="7">
-        <v>0.49767060276937197</v>
+        <v>0.55414240668196202</v>
       </c>
       <c r="F656" s="7">
-        <v>0.51167307318335098</v>
+        <v>0.56448715371681901</v>
       </c>
       <c r="G656" s="7">
-        <v>1.9612258751781999</v>
+        <v>1.9168093156658099</v>
       </c>
     </row>
     <row r="657" spans="1:7">
@@ -15591,13 +15591,13 @@
         <v>1369</v>
       </c>
       <c r="E657" s="7">
-        <v>0.51437667009509702</v>
+        <v>0.55393518503174699</v>
       </c>
       <c r="F657" s="7">
-        <v>0.53265709099248904</v>
+        <v>0.56045559393412103</v>
       </c>
       <c r="G657" s="7">
-        <v>1.93993527510985</v>
+        <v>1.90961229645135</v>
       </c>
     </row>
     <row r="658" spans="1:7">
@@ -15614,13 +15614,13 @@
         <v>1389</v>
       </c>
       <c r="E658" s="7">
-        <v>0.515166303032627</v>
+        <v>0.56628661823260995</v>
       </c>
       <c r="F658" s="7">
-        <v>0.53248067990605197</v>
+        <v>0.579606716739684</v>
       </c>
       <c r="G658" s="7">
-        <v>1.9369470403854501</v>
+        <v>1.89337876459801</v>
       </c>
     </row>
     <row r="659" spans="1:7">
@@ -15637,13 +15637,13 @@
         <v>1404</v>
       </c>
       <c r="E659" s="7">
-        <v>0.52974284539624406</v>
+        <v>0.56703695714824098</v>
       </c>
       <c r="F659" s="7">
-        <v>0.54191786380525198</v>
+        <v>0.57865183104245699</v>
       </c>
       <c r="G659" s="7">
-        <v>1.91331962141798</v>
+        <v>1.88824335027777</v>
       </c>
     </row>
     <row r="660" spans="1:7">
@@ -15660,13 +15660,13 @@
         <v>1419</v>
       </c>
       <c r="E660" s="7">
-        <v>0.53223562996793805</v>
+        <v>0.57541651999868904</v>
       </c>
       <c r="F660" s="7">
-        <v>0.54729273736540296</v>
+        <v>0.58394659131106197</v>
       </c>
       <c r="G660" s="7">
-        <v>1.90977617437493</v>
+        <v>1.8799301554191801</v>
       </c>
     </row>
     <row r="661" spans="1:7">
@@ -15683,13 +15683,13 @@
         <v>1425</v>
       </c>
       <c r="E661" s="7">
-        <v>0.536206624524735</v>
+        <v>0.57423535477871102</v>
       </c>
       <c r="F661" s="7">
-        <v>0.55063402808052897</v>
+        <v>0.58561035825470398</v>
       </c>
       <c r="G661" s="7">
-        <v>1.9052494442339001</v>
+        <v>1.8777048170030599</v>
       </c>
     </row>
     <row r="662" spans="1:7">
@@ -15706,13 +15706,13 @@
         <v>1441</v>
       </c>
       <c r="E662" s="7">
-        <v>0.53147914752832204</v>
+        <v>0.56846099168706699</v>
       </c>
       <c r="F662" s="7">
-        <v>0.54421039870376298</v>
+        <v>0.57761764127885096</v>
       </c>
       <c r="G662" s="7">
-        <v>1.90940087824981</v>
+        <v>1.88475809669554</v>
       </c>
     </row>
     <row r="663" spans="1:7">
@@ -15729,13 +15729,13 @@
         <v>1458</v>
       </c>
       <c r="E663" s="7">
-        <v>0.52567314172744095</v>
+        <v>0.56571103655621002</v>
       </c>
       <c r="F663" s="7">
-        <v>0.53932267869423001</v>
+        <v>0.57878697164536996</v>
       </c>
       <c r="G663" s="7">
-        <v>1.9159971034263099</v>
+        <v>1.8841525044424701</v>
       </c>
     </row>
     <row r="664" spans="1:7">
@@ -15752,13 +15752,13 @@
         <v>1474</v>
       </c>
       <c r="E664" s="7">
-        <v>0.53506984543970604</v>
+        <v>0.57402836003957902</v>
       </c>
       <c r="F664" s="7">
-        <v>0.55237305296471595</v>
+        <v>0.58314060304458903</v>
       </c>
       <c r="G664" s="7">
-        <v>1.90312193346564</v>
+        <v>1.8710046475403801</v>
       </c>
     </row>
     <row r="665" spans="1:7">
@@ -15775,13 +15775,13 @@
         <v>1489</v>
       </c>
       <c r="E665" s="7">
-        <v>0.53854568842527295</v>
+        <v>0.57491472167856705</v>
       </c>
       <c r="F665" s="7">
-        <v>0.55371151139116703</v>
+        <v>0.58527291136000603</v>
       </c>
       <c r="G665" s="7">
-        <v>1.8992419505157001</v>
+        <v>1.8708092114116099</v>
       </c>
     </row>
     <row r="666" spans="1:7">
@@ -15798,13 +15798,13 @@
         <v>1527</v>
       </c>
       <c r="E666" s="7">
-        <v>0.535752829096245</v>
+        <v>0.56991511776180603</v>
       </c>
       <c r="F666" s="7">
-        <v>0.553265628324072</v>
+        <v>0.576953267416628</v>
       </c>
       <c r="G666" s="7">
-        <v>1.89958859265145</v>
+        <v>1.87316524221809</v>
       </c>
     </row>
     <row r="667" spans="1:7">
@@ -15821,13 +15821,13 @@
         <v>1559</v>
       </c>
       <c r="E667" s="7">
-        <v>0.55797841168502804</v>
+        <v>0.58632937035558697</v>
       </c>
       <c r="F667" s="7">
-        <v>0.56824276771752102</v>
+        <v>0.59455472402711496</v>
       </c>
       <c r="G667" s="7">
-        <v>1.8670734252724199</v>
+        <v>1.8481040138429801</v>
       </c>
     </row>
     <row r="668" spans="1:7">
@@ -15844,13 +15844,13 @@
         <v>1608</v>
       </c>
       <c r="E668" s="7">
-        <v>0.55136839544664795</v>
+        <v>0.58510325455527801</v>
       </c>
       <c r="F668" s="7">
-        <v>0.56393849905349702</v>
+        <v>0.59616427288455898</v>
       </c>
       <c r="G668" s="7">
-        <v>1.8780706957467901</v>
+        <v>1.8496375008635799</v>
       </c>
     </row>
     <row r="669" spans="1:7">
@@ -15867,13 +15867,13 @@
         <v>1667</v>
       </c>
       <c r="E669" s="7">
-        <v>0.55106047608612396</v>
+        <v>0.57968170826247301</v>
       </c>
       <c r="F669" s="7">
-        <v>0.56234999005039898</v>
+        <v>0.58831236108778895</v>
       </c>
       <c r="G669" s="7">
-        <v>1.87643609802403</v>
+        <v>1.8548657023254</v>
       </c>
     </row>
     <row r="670" spans="1:7">
@@ -15890,13 +15890,13 @@
         <v>1749</v>
       </c>
       <c r="E670" s="7">
-        <v>0.55260226073304197</v>
+        <v>0.58150347795745405</v>
       </c>
       <c r="F670" s="7">
-        <v>0.56453004265067697</v>
+        <v>0.57994659130988302</v>
       </c>
       <c r="G670" s="7">
-        <v>1.8752518318979801</v>
+        <v>1.8553391448304599</v>
       </c>
     </row>
     <row r="671" spans="1:7">
@@ -15913,13 +15913,13 @@
         <v>1905</v>
       </c>
       <c r="E671" s="7">
-        <v>0.553354078623018</v>
+        <v>0.59174708573768398</v>
       </c>
       <c r="F671" s="7">
-        <v>0.56481003455850798</v>
+        <v>0.59282460061976805</v>
       </c>
       <c r="G671" s="7">
-        <v>1.8731399232330099</v>
+        <v>1.8361101737332299</v>
       </c>
     </row>
     <row r="672" spans="1:7">
@@ -15936,13 +15936,13 @@
         <v>2764</v>
       </c>
       <c r="E672" s="7">
-        <v>0.54910885940423104</v>
+        <v>0.59445272241815705</v>
       </c>
       <c r="F672" s="7">
-        <v>0.55901598236177696</v>
+        <v>0.59563989497625203</v>
       </c>
       <c r="G672" s="7">
-        <v>1.87912885678383</v>
+        <v>1.82866122335157</v>
       </c>
     </row>
     <row r="673" spans="1:7">

</xml_diff>